<commit_message>
Add documents : analytical matching functions formulas and link to reference paper
</commit_message>
<xml_diff>
--- a/Docs/Curves/snake-curves-from-paper.xlsx
+++ b/Docs/Curves/snake-curves-from-paper.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RGB" sheetId="1" r:id="rId1"/>
     <sheet name="CMY" sheetId="2" r:id="rId2"/>
     <sheet name="W" sheetId="3" r:id="rId3"/>
+    <sheet name="matching-functions" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t>R</t>
     <phoneticPr fontId="1"/>
@@ -161,22 +162,55 @@
     <t>formula W</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>x-param-1</t>
+  </si>
+  <si>
+    <t>x-param-2</t>
+  </si>
+  <si>
+    <t>x-param-3</t>
+  </si>
+  <si>
+    <t>y-param-1</t>
+  </si>
+  <si>
+    <t>y-param-2</t>
+  </si>
+  <si>
+    <t>z-param-1</t>
+  </si>
+  <si>
+    <t>z-param-2</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -202,11 +236,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -217,9 +253,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -227,7 +260,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -239,6 +272,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -264,7 +298,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ja-JP"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -844,11 +878,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="233311776"/>
-        <c:axId val="233312336"/>
+        <c:axId val="168866176"/>
+        <c:axId val="168868096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="233311776"/>
+        <c:axId val="168866176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -902,15 +936,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="233312336"/>
+        <c:crossAx val="168868096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="233312336"/>
+        <c:axId val="168868096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -964,10 +998,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="233311776"/>
+        <c:crossAx val="168866176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -981,6 +1015,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1006,7 +1041,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ja-JP"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1036,7 +1071,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="ja-JP"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1050,7 +1085,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1088,7 +1123,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ja-JP"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1658,11 +1693,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="233316256"/>
-        <c:axId val="233316816"/>
+        <c:axId val="169315328"/>
+        <c:axId val="163959168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="233316256"/>
+        <c:axId val="169315328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1716,15 +1751,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="233316816"/>
+        <c:crossAx val="163959168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="233316816"/>
+        <c:axId val="163959168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1778,10 +1813,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="233316256"/>
+        <c:crossAx val="169315328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1821,7 +1856,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ja-JP"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1851,7 +1886,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="ja-JP"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1865,7 +1900,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1903,7 +1938,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ja-JP"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2105,11 +2140,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="313510784"/>
-        <c:axId val="313509104"/>
+        <c:axId val="164251520"/>
+        <c:axId val="164278272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="313510784"/>
+        <c:axId val="164251520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2163,15 +2198,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313509104"/>
+        <c:crossAx val="164278272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="313509104"/>
+        <c:axId val="164278272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2225,10 +2260,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313510784"/>
+        <c:crossAx val="164251520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2266,9 +2301,569 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="ja-JP"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'matching-functions'!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>x</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'matching-functions'!$C$2:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>361.85567010309279</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>383.50515463917526</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>405.15463917525773</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>426.8041237113402</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>448.45360824742266</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>470.10309278350519</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>491.75257731958766</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>513.40206185567013</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>535.05154639175259</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>556.70103092783506</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>578.35051546391753</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>621.64948453608247</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>643.29896907216494</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>664.94845360824741</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>686.59793814432987</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>708.24742268041246</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>729.89690721649481</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>751.54639175257739</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>773.19587628865975</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>794.84536082474233</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'matching-functions'!$O$2:$O$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1.3451238348390995E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6314693711256344E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.575511594613691E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23086736416042122</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.34963547426308383</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1908584697796481</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3638828744004574E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.036622755221919E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.21782424288811711</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.54598970279762771</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.89873331791006006</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0559262692943967</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.82320741591236335</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.39354972842347435</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.11537810797992082</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.0743471151246917E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.2870396774107324E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.5463230015408432E-4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.4115197203944047E-6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.6302567166576535E-7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.5420568769439531E-9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'matching-functions'!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'matching-functions'!$C$2:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>361.85567010309279</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>383.50515463917526</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>405.15463917525773</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>426.8041237113402</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>448.45360824742266</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>470.10309278350519</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>491.75257731958766</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>513.40206185567013</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>535.05154639175259</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>556.70103092783506</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>578.35051546391753</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>621.64948453608247</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>643.29896907216494</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>664.94845360824741</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>686.59793814432987</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>708.24742268041246</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>729.89690721649481</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>751.54639175257739</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>773.19587628865975</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>794.84536082474233</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'matching-functions'!$P$2:$P$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>4.9571916461377961E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4027067045260781E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.888265048999064E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.4713191478562513E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0725588255346513E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.0365513055816041E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.22962128259108247</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.57015192084641264</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.91752390014029428</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99671398035690228</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.88748091986574262</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.6341359279753237</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.35420360402147127</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.15144156372921619</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.896241207285517E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.1913762710001084E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.1787600197033319E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.9937188905645307E-4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.0905103453674714E-5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.3969755519380043E-6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.3967248013124575E-7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'matching-functions'!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>z</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'matching-functions'!$C$2:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>361.85567010309279</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>383.50515463917526</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>405.15463917525773</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>426.8041237113402</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>448.45360824742266</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>470.10309278350519</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>491.75257731958766</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>513.40206185567013</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>535.05154639175259</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>556.70103092783506</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>578.35051546391753</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>621.64948453608247</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>643.29896907216494</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>664.94845360824741</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>686.59793814432987</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>708.24742268041246</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>729.89690721649481</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>751.54639175257739</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>773.19587628865975</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>794.84536082474233</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'matching-functions'!$Q$2:$Q$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>6.2472337113960667E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0014099553852381E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.11200034671829542</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1555397701091339</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7839595686535503</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2894136948601176</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.42273442181613835</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.12783465826256846</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.9638289810620437E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.7941105054857278E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.3982232177091311E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.2313508796912072E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.3088336524122852E-6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.769839591965497E-8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.318868163505933E-9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.2682108802515279E-11</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.4689138398488195E-13</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.8779988812652566E-15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.0287798943825876E-17</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.3091190217792603E-19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.938909069675296E-22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="168842752"/>
+        <c:axId val="168841216"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="168842752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="168841216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="168841216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="168842752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -4050,6 +4645,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4093,7 +4723,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4128,7 +4758,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4340,25 +4970,24 @@
   <dimension ref="A2:H72"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA33" sqref="AA33:AC54"/>
+      <selection activeCell="A51" sqref="A51:C72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" customWidth="1"/>
-    <col min="7" max="7" width="9.21875" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="7" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -4379,7 +5008,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>19</v>
       </c>
@@ -4399,7 +5028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>58</v>
       </c>
@@ -4421,7 +5050,7 @@
         <v>0.20588235294117646</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="B6">
         <v>18</v>
       </c>
@@ -4437,7 +5066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>397</v>
       </c>
@@ -4449,7 +5078,7 @@
         <v>749.48453608247428</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>446</v>
       </c>
@@ -4461,12 +5090,12 @@
         <v>800</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="45">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -4489,7 +5118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>19</v>
       </c>
@@ -4517,7 +5146,7 @@
         <v>9.5588235294117641E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>62</v>
       </c>
@@ -4545,7 +5174,7 @@
         <v>8.8235294117647065E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>83</v>
       </c>
@@ -4573,7 +5202,7 @@
         <v>7.3529411764705885E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>89</v>
       </c>
@@ -4601,7 +5230,7 @@
         <v>6.6176470588235295E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>105</v>
       </c>
@@ -4629,7 +5258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>211</v>
       </c>
@@ -4657,7 +5286,7 @@
         <v>8.8235294117647065E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>233</v>
       </c>
@@ -4685,7 +5314,7 @@
         <v>0.69852941176470584</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>254</v>
       </c>
@@ -4712,12 +5341,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="45">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
@@ -4740,7 +5369,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>19</v>
       </c>
@@ -4767,7 +5396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>105</v>
       </c>
@@ -4794,7 +5423,7 @@
         <v>3.6764705882352942E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>126</v>
       </c>
@@ -4821,7 +5450,7 @@
         <v>0.38970588235294118</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>147</v>
       </c>
@@ -4848,7 +5477,7 @@
         <v>0.78676470588235292</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>169</v>
       </c>
@@ -4875,7 +5504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>211</v>
       </c>
@@ -4902,7 +5531,7 @@
         <v>0.77941176470588236</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>233</v>
       </c>
@@ -4929,7 +5558,7 @@
         <v>0.31617647058823528</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>254</v>
       </c>
@@ -4956,7 +5585,7 @@
         <v>7.3529411764705881E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8">
       <c r="A33">
         <v>275</v>
       </c>
@@ -4979,12 +5608,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="45">
       <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
@@ -5007,7 +5636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8">
       <c r="A38">
         <v>19</v>
       </c>
@@ -5034,7 +5663,7 @@
         <v>0.99264705882352944</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8">
       <c r="A39">
         <v>43</v>
       </c>
@@ -5061,7 +5690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8">
       <c r="A40">
         <v>105</v>
       </c>
@@ -5088,7 +5717,7 @@
         <v>0.86764705882352944</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8">
       <c r="A41">
         <v>126</v>
       </c>
@@ -5115,7 +5744,7 @@
         <v>0.61029411764705888</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8">
       <c r="A42">
         <v>147</v>
       </c>
@@ -5142,7 +5771,7 @@
         <v>0.30882352941176472</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8">
       <c r="A43">
         <v>169</v>
       </c>
@@ -5169,7 +5798,7 @@
         <v>8.0882352941176475E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8">
       <c r="A44">
         <v>190</v>
       </c>
@@ -5196,7 +5825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8">
       <c r="A45">
         <v>254</v>
       </c>
@@ -5223,7 +5852,7 @@
         <v>2.9411764705882353E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8">
       <c r="A46">
         <v>275</v>
       </c>
@@ -5250,7 +5879,7 @@
         <v>5.1470588235294115E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8">
       <c r="A47">
         <v>298</v>
       </c>
@@ -5277,12 +5906,12 @@
         <v>6.6176470588235295E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" ht="30">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -5302,7 +5931,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6">
       <c r="A52">
         <v>1</v>
       </c>
@@ -5327,7 +5956,7 @@
         <v>0.99264705882352944</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6">
       <c r="A53">
         <v>2</v>
       </c>
@@ -5352,7 +5981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6">
       <c r="A54">
         <v>3</v>
       </c>
@@ -5377,7 +6006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6">
       <c r="A55">
         <v>4</v>
       </c>
@@ -5402,7 +6031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6">
       <c r="A56">
         <v>5</v>
       </c>
@@ -5427,7 +6056,7 @@
         <v>0.86764705882352944</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6">
       <c r="A57">
         <v>6</v>
       </c>
@@ -5452,7 +6081,7 @@
         <v>0.61029411764705888</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6">
       <c r="A58">
         <v>7</v>
       </c>
@@ -5477,7 +6106,7 @@
         <v>0.30882352941176472</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6">
       <c r="A59">
         <v>8</v>
       </c>
@@ -5502,7 +6131,7 @@
         <v>8.0882352941176475E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6">
       <c r="A60">
         <v>9</v>
       </c>
@@ -5527,7 +6156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6">
       <c r="A61">
         <v>10</v>
       </c>
@@ -5552,7 +6181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6">
       <c r="A62">
         <v>11</v>
       </c>
@@ -5577,7 +6206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6">
       <c r="A63">
         <v>12</v>
       </c>
@@ -5602,7 +6231,7 @@
         <v>2.9411764705882353E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6">
       <c r="A64">
         <v>13</v>
       </c>
@@ -5627,7 +6256,7 @@
         <v>5.1470588235294115E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6">
       <c r="A65">
         <v>14</v>
       </c>
@@ -5652,7 +6281,7 @@
         <v>6.6176470588235295E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6">
       <c r="A66">
         <v>15</v>
       </c>
@@ -5677,7 +6306,7 @@
         <v>6.6176470588235295E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6">
       <c r="A67">
         <v>16</v>
       </c>
@@ -5702,7 +6331,7 @@
         <v>6.6176470588235295E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6">
       <c r="A68">
         <v>17</v>
       </c>
@@ -5727,7 +6356,7 @@
         <v>6.6176470588235295E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6">
       <c r="A69">
         <v>18</v>
       </c>
@@ -5752,7 +6381,7 @@
         <v>6.6176470588235295E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6">
       <c r="A70">
         <v>19</v>
       </c>
@@ -5777,7 +6406,7 @@
         <v>6.6176470588235295E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6">
       <c r="A71">
         <v>20</v>
       </c>
@@ -5802,7 +6431,7 @@
         <v>6.6176470588235295E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6">
       <c r="A72">
         <v>21</v>
       </c>
@@ -5840,17 +6469,17 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:I23"/>
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="45">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -5879,7 +6508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5913,7 +6542,7 @@
         <v>7.3529411764705881E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>2</v>
       </c>
@@ -5947,7 +6576,7 @@
         <v>7.3529411764705881E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>3</v>
       </c>
@@ -5981,7 +6610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>4</v>
       </c>
@@ -6015,7 +6644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>5</v>
       </c>
@@ -6049,7 +6678,7 @@
         <v>0.3014705882352941</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>6</v>
       </c>
@@ -6083,7 +6712,7 @@
         <v>0.39705882352941174</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>7</v>
       </c>
@@ -6117,7 +6746,7 @@
         <v>0.69852941176470584</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>8</v>
       </c>
@@ -6151,7 +6780,7 @@
         <v>0.92647058823529416</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>9</v>
       </c>
@@ -6185,7 +6814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>10</v>
       </c>
@@ -6219,7 +6848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>11</v>
       </c>
@@ -6253,7 +6882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>12</v>
       </c>
@@ -6287,7 +6916,7 @@
         <v>0.97058823529411764</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>13</v>
       </c>
@@ -6321,7 +6950,7 @@
         <v>0.95588235294117652</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>14</v>
       </c>
@@ -6355,7 +6984,7 @@
         <v>0.95588235294117652</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>15</v>
       </c>
@@ -6389,7 +7018,7 @@
         <v>0.95588235294117652</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>16</v>
       </c>
@@ -6423,7 +7052,7 @@
         <v>0.96323529411764708</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>17</v>
       </c>
@@ -6457,7 +7086,7 @@
         <v>0.97058823529411764</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>18</v>
       </c>
@@ -6491,7 +7120,7 @@
         <v>0.98529411764705888</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>19</v>
       </c>
@@ -6525,7 +7154,7 @@
         <v>0.99264705882352944</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>20</v>
       </c>
@@ -6559,7 +7188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>21</v>
       </c>
@@ -6605,18 +7234,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:E29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="30">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -6627,7 +7256,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>154</v>
       </c>
@@ -6639,7 +7268,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>42</v>
       </c>
@@ -6651,12 +7280,12 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="45">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -6673,7 +7302,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>1</v>
       </c>
@@ -6685,7 +7314,7 @@
         <v>84</v>
       </c>
       <c r="D9">
-        <f>400+(800-400)*(B9-58)/(446-58)</f>
+        <f t="shared" ref="D9:D29" si="0">400+(800-400)*(B9-58)/(446-58)</f>
         <v>361.85567010309279</v>
       </c>
       <c r="E9">
@@ -6693,403 +7322,403 @@
         <v>0.98750000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10">
-        <f t="shared" ref="B10:B29" si="0">21*A10</f>
+        <f t="shared" ref="B10:B29" si="1">21*A10</f>
         <v>42</v>
       </c>
       <c r="C10">
         <v>81</v>
       </c>
       <c r="D10">
-        <f>400+(800-400)*(B10-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>383.50515463917526</v>
       </c>
       <c r="E10">
-        <f t="shared" ref="E10:E29" si="1">0.8+(1.1-0.8)*(154-C10)/(154-42)</f>
+        <f t="shared" ref="E10:E29" si="2">0.8+(1.1-0.8)*(154-C10)/(154-42)</f>
         <v>0.99553571428571441</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>3</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="C11">
         <v>58</v>
       </c>
       <c r="D11">
-        <f>400+(800-400)*(B11-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>405.15463917525773</v>
       </c>
       <c r="E11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0571428571428572</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>4</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="C12">
         <v>51</v>
       </c>
       <c r="D12">
-        <f>400+(800-400)*(B12-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>426.8041237113402</v>
       </c>
       <c r="E12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0758928571428572</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>5</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
       <c r="C13">
         <v>118</v>
       </c>
       <c r="D13">
-        <f>400+(800-400)*(B13-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>448.45360824742266</v>
       </c>
       <c r="E13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.89642857142857146</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>6</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>126</v>
       </c>
       <c r="C14">
         <v>81</v>
       </c>
       <c r="D14">
-        <f>400+(800-400)*(B14-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>470.10309278350519</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99553571428571441</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>7</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>147</v>
       </c>
       <c r="C15">
         <v>36</v>
       </c>
       <c r="D15">
-        <f>400+(800-400)*(B15-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>491.75257731958766</v>
       </c>
       <c r="E15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.1160714285714286</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>8</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>168</v>
       </c>
       <c r="C16">
         <v>50</v>
       </c>
       <c r="D16">
-        <f>400+(800-400)*(B16-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>513.40206185567013</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0785714285714287</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>9</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>189</v>
       </c>
       <c r="C17">
         <v>79</v>
       </c>
       <c r="D17">
-        <f>400+(800-400)*(B17-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>535.05154639175259</v>
       </c>
       <c r="E17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0008928571428573</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>10</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>210</v>
       </c>
       <c r="C18">
         <v>138</v>
       </c>
       <c r="D18">
-        <f>400+(800-400)*(B18-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>556.70103092783506</v>
       </c>
       <c r="E18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.84285714285714286</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>11</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>231</v>
       </c>
       <c r="C19">
         <v>72</v>
       </c>
       <c r="D19">
-        <f>400+(800-400)*(B19-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>578.35051546391753</v>
       </c>
       <c r="E19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0196428571428573</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>12</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>252</v>
       </c>
       <c r="C20">
         <v>62</v>
       </c>
       <c r="D20">
-        <f>400+(800-400)*(B20-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="E20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0464285714285715</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>13</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>273</v>
       </c>
       <c r="C21">
         <v>60</v>
       </c>
       <c r="D21">
-        <f>400+(800-400)*(B21-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>621.64948453608247</v>
       </c>
       <c r="E21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0517857142857143</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>14</v>
       </c>
       <c r="B22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>294</v>
       </c>
       <c r="C22">
         <v>56</v>
       </c>
       <c r="D22">
-        <f>400+(800-400)*(B22-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>643.29896907216494</v>
       </c>
       <c r="E22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0625</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>15</v>
       </c>
       <c r="B23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>315</v>
       </c>
       <c r="C23">
         <v>55</v>
       </c>
       <c r="D23">
-        <f>400+(800-400)*(B23-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>664.94845360824741</v>
       </c>
       <c r="E23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0651785714285715</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>16</v>
       </c>
       <c r="B24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>336</v>
       </c>
       <c r="C24">
         <v>55</v>
       </c>
       <c r="D24">
-        <f>400+(800-400)*(B24-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>686.59793814432987</v>
       </c>
       <c r="E24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0651785714285715</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>17</v>
       </c>
       <c r="B25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>357</v>
       </c>
       <c r="C25">
         <v>56</v>
       </c>
       <c r="D25">
-        <f>400+(800-400)*(B25-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>708.24742268041246</v>
       </c>
       <c r="E25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0625</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>18</v>
       </c>
       <c r="B26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>378</v>
       </c>
       <c r="C26">
         <v>55</v>
       </c>
       <c r="D26">
-        <f>400+(800-400)*(B26-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>729.89690721649481</v>
       </c>
       <c r="E26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0651785714285715</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>19</v>
       </c>
       <c r="B27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>399</v>
       </c>
       <c r="C27">
         <v>54</v>
       </c>
       <c r="D27">
-        <f>400+(800-400)*(B27-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>751.54639175257739</v>
       </c>
       <c r="E27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0678571428571431</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>20</v>
       </c>
       <c r="B28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>420</v>
       </c>
       <c r="C28">
         <v>54</v>
       </c>
       <c r="D28">
-        <f>400+(800-400)*(B28-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>773.19587628865975</v>
       </c>
       <c r="E28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0678571428571431</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>21</v>
       </c>
       <c r="B29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>441</v>
       </c>
       <c r="C29">
         <v>55</v>
       </c>
       <c r="D29">
-        <f>400+(800-400)*(B29-58)/(446-58)</f>
+        <f t="shared" si="0"/>
         <v>794.84536082474233</v>
       </c>
       <c r="E29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0651785714285715</v>
       </c>
     </row>
@@ -7098,4 +7727,1247 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" customWidth="1"/>
+    <col min="9" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.42578125" customWidth="1"/>
+    <col min="12" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.42578125" customWidth="1"/>
+    <col min="15" max="16" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="45">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="3"/>
+      <c r="O1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>21*A2</f>
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <f>400+(800-400)*(B2-58)/(446-58)</f>
+        <v>361.85567010309279</v>
+      </c>
+      <c r="E2">
+        <f>(C2-442)*IF(C2 &lt; 442,0.0624,0.0374)</f>
+        <v>-5.00100618556701</v>
+      </c>
+      <c r="F2">
+        <f>(C2-599.8)*IF(C2 &lt; 599.8,0.0264,0.0323)</f>
+        <v>-6.2817303092783492</v>
+      </c>
+      <c r="G2">
+        <f>(C2-501.1)*IF(C2 &lt; 501.1,0.049,0.0382)</f>
+        <v>-6.8229721649484549</v>
+      </c>
+      <c r="I2">
+        <f>(C2-568.8)*IF(C2 &lt; 568.8,0.0213,0.0247)</f>
+        <v>-4.407914226804122</v>
+      </c>
+      <c r="J2">
+        <f>(C2-530.9)*IF(C2 &lt; 530.9,0.0613,0.0322)</f>
+        <v>-10.36241742268041</v>
+      </c>
+      <c r="L2">
+        <f>(C2-437)*IF(C2 &lt; 437,0.0845,0.0278)</f>
+        <v>-6.3496958762886599</v>
+      </c>
+      <c r="M2">
+        <f>(C2-459)*IF(C2 &lt; 459,0.0385,0.0725)</f>
+        <v>-3.7400567010309276</v>
+      </c>
+      <c r="O2" s="2">
+        <f>0.362*EXP(-0.5*E2*E2) + 1.056*EXP(-0.5*F2*F2) - 0.065*EXP(-0.5*G2*G2)</f>
+        <v>1.3451238348390995E-6</v>
+      </c>
+      <c r="P2" s="2">
+        <f>0.821*EXP(-0.5*I2*I2) + 0.286*EXP(-0.5*J2*J2)</f>
+        <v>4.9571916461377961E-5</v>
+      </c>
+      <c r="Q2" s="2">
+        <f>1.217*EXP(-0.5*L2*L2) + 0.681*EXP(-0.5*M2*M2)</f>
+        <v>6.2472337113960667E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B22" si="0">21*A3</f>
+        <v>42</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C22" si="1">400+(800-400)*(B3-58)/(446-58)</f>
+        <v>383.50515463917526</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E22" si="2">(C3-442)*IF(C3 &lt; 442,0.0624,0.0374)</f>
+        <v>-3.6500783505154635</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F22" si="3">(C3-599.8)*IF(C3 &lt; 599.8,0.0264,0.0323)</f>
+        <v>-5.7101839175257716</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G22" si="4">(C3-501.1)*IF(C3 &lt; 501.1,0.049,0.0382)</f>
+        <v>-5.7621474226804139</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3">
+        <f t="shared" ref="I3:I22" si="5">(C3-568.8)*IF(C3 &lt; 568.8,0.0213,0.0247)</f>
+        <v>-3.9467802061855659</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" ref="J3:J22" si="6">(C3-530.9)*IF(C3 &lt; 530.9,0.0613,0.0322)</f>
+        <v>-9.0353040206185558</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f t="shared" ref="L3:L22" si="7">(C3-437)*IF(C3 &lt; 437,0.0845,0.0278)</f>
+        <v>-4.5203144329896912</v>
+      </c>
+      <c r="M3" s="3">
+        <f t="shared" ref="M3:M22" si="8">(C3-459)*IF(C3 &lt; 459,0.0385,0.0725)</f>
+        <v>-2.9065515463917526</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="2">
+        <f t="shared" ref="O3:O22" si="9">0.362*EXP(-0.5*E3*E3) + 1.056*EXP(-0.5*F3*F3) - 0.065*EXP(-0.5*G3*G3)</f>
+        <v>4.6314693711256344E-4</v>
+      </c>
+      <c r="P3" s="2">
+        <f t="shared" ref="P3:P22" si="10">0.821*EXP(-0.5*I3*I3) + 0.286*EXP(-0.5*J3*J3)</f>
+        <v>3.4027067045260781E-4</v>
+      </c>
+      <c r="Q3" s="2">
+        <f t="shared" ref="Q3:Q22" si="11">1.217*EXP(-0.5*L3*L3) + 0.681*EXP(-0.5*M3*M3)</f>
+        <v>1.0014099553852381E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>405.15463917525773</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="2"/>
+        <v>-2.2991505154639178</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="3"/>
+        <v>-5.1386375257731949</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="4"/>
+        <v>-4.7013226804123729</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3">
+        <f t="shared" si="5"/>
+        <v>-3.4856461855670093</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="6"/>
+        <v>-7.7081906185567002</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3">
+        <f t="shared" si="7"/>
+        <v>-2.6909329896907224</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" si="8"/>
+        <v>-2.0730463917525777</v>
+      </c>
+      <c r="N4" s="3"/>
+      <c r="O4" s="2">
+        <f t="shared" si="9"/>
+        <v>2.575511594613691E-2</v>
+      </c>
+      <c r="P4" s="2">
+        <f t="shared" si="10"/>
+        <v>1.888265048999064E-3</v>
+      </c>
+      <c r="Q4" s="2">
+        <f t="shared" si="11"/>
+        <v>0.11200034671829542</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>426.8041237113402</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.94822268041237168</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="3"/>
+        <v>-4.5670911340206173</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="4"/>
+        <v>-3.6404979381443314</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3">
+        <f t="shared" si="5"/>
+        <v>-3.0245121649484528</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="6"/>
+        <v>-6.3810772164948446</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3">
+        <f t="shared" si="7"/>
+        <v>-0.86155154639175346</v>
+      </c>
+      <c r="M5" s="3">
+        <f t="shared" si="8"/>
+        <v>-1.2395412371134025</v>
+      </c>
+      <c r="N5" s="3"/>
+      <c r="O5" s="2">
+        <f t="shared" si="9"/>
+        <v>0.23086736416042122</v>
+      </c>
+      <c r="P5" s="2">
+        <f t="shared" si="10"/>
+        <v>8.4713191478562513E-3</v>
+      </c>
+      <c r="Q5" s="2">
+        <f t="shared" si="11"/>
+        <v>1.1555397701091339</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>448.45360824742266</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="2"/>
+        <v>0.24136494845360768</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="3"/>
+        <v>-3.9955447422680406</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="4"/>
+        <v>-2.5796731958762908</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3">
+        <f t="shared" si="5"/>
+        <v>-2.5633781443298962</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="6"/>
+        <v>-5.053963814432989</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3">
+        <f t="shared" si="7"/>
+        <v>0.31841030927835007</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="shared" si="8"/>
+        <v>-0.4060360824742274</v>
+      </c>
+      <c r="N6" s="3"/>
+      <c r="O6" s="2">
+        <f t="shared" si="9"/>
+        <v>0.34963547426308383</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" si="10"/>
+        <v>3.0725588255346513E-2</v>
+      </c>
+      <c r="Q6" s="2">
+        <f t="shared" si="11"/>
+        <v>1.7839595686535503</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>470.10309278350519</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0510556701030942</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="3"/>
+        <v>-3.4239983505154616</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="4"/>
+        <v>-1.5188484536082469</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3">
+        <f t="shared" si="5"/>
+        <v>-2.1022441237113383</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="6"/>
+        <v>-3.7268504123711303</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3">
+        <f t="shared" si="7"/>
+        <v>0.92026597938144417</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" si="8"/>
+        <v>0.80497422680412622</v>
+      </c>
+      <c r="N7" s="3"/>
+      <c r="O7" s="2">
+        <f t="shared" si="9"/>
+        <v>0.1908584697796481</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" si="10"/>
+        <v>9.0365513055816041E-2</v>
+      </c>
+      <c r="Q7" s="2">
+        <f t="shared" si="11"/>
+        <v>1.2894136948601176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>147</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>491.75257731958766</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="2"/>
+        <v>1.8607463917525786</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="3"/>
+        <v>-2.8524519587628845</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.45802371134020586</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3">
+        <f t="shared" si="5"/>
+        <v>-1.6411101030927819</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="6"/>
+        <v>-2.3997370103092752</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3">
+        <f t="shared" si="7"/>
+        <v>1.5221216494845369</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="8"/>
+        <v>2.3745618556701049</v>
+      </c>
+      <c r="N8" s="3"/>
+      <c r="O8" s="2">
+        <f t="shared" si="9"/>
+        <v>2.3638828744004574E-2</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="10"/>
+        <v>0.22962128259108247</v>
+      </c>
+      <c r="Q8" s="2">
+        <f t="shared" si="11"/>
+        <v>0.42273442181613835</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>168</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>513.40206185567013</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="2"/>
+        <v>2.670437113402063</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="3"/>
+        <v>-2.2809055670103073</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="4"/>
+        <v>0.46993876288659792</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3">
+        <f t="shared" si="5"/>
+        <v>-1.1799760824742254</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="6"/>
+        <v>-1.0726236082474199</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3">
+        <f t="shared" si="7"/>
+        <v>2.1239773195876293</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" si="8"/>
+        <v>3.944149484536084</v>
+      </c>
+      <c r="N9" s="3"/>
+      <c r="O9" s="2">
+        <f t="shared" si="9"/>
+        <v>3.036622755221919E-2</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="10"/>
+        <v>0.57015192084641264</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" si="11"/>
+        <v>0.12783465826256846</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>189</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>535.05154639175259</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="2"/>
+        <v>3.4801278350515474</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="3"/>
+        <v>-1.7093591752577302</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="4"/>
+        <v>1.2969490721649481</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3">
+        <f t="shared" si="5"/>
+        <v>-0.71884206185566879</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="6"/>
+        <v>0.13367979381443429</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3">
+        <f t="shared" si="7"/>
+        <v>2.7258329896907219</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" si="8"/>
+        <v>5.5137371134020627</v>
+      </c>
+      <c r="N10" s="3"/>
+      <c r="O10" s="2">
+        <f t="shared" si="9"/>
+        <v>0.21782424288811711</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="10"/>
+        <v>0.91752390014029428</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" si="11"/>
+        <v>2.9638289810620437E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>556.70103092783506</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="2"/>
+        <v>4.2898185567010314</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="3"/>
+        <v>-1.137812783505153</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="4"/>
+        <v>2.1239593814432984</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3">
+        <f t="shared" si="5"/>
+        <v>-0.25770804123711216</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="6"/>
+        <v>0.83079319587628975</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3">
+        <f t="shared" si="7"/>
+        <v>3.3276886597938145</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" si="8"/>
+        <v>7.0833247422680419</v>
+      </c>
+      <c r="N11" s="3"/>
+      <c r="O11" s="2">
+        <f t="shared" si="9"/>
+        <v>0.54598970279762771</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" si="10"/>
+        <v>0.99671398035690228</v>
+      </c>
+      <c r="Q11" s="2">
+        <f t="shared" si="11"/>
+        <v>4.7941105054857278E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>231</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>578.35051546391753</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="2"/>
+        <v>5.0995092783505163</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="3"/>
+        <v>-0.56626639175257598</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="4"/>
+        <v>2.9509696907216485</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3">
+        <f t="shared" si="5"/>
+        <v>0.23589773195876415</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="6"/>
+        <v>1.5279065979381452</v>
+      </c>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3">
+        <f t="shared" si="7"/>
+        <v>3.9295443298969071</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="8"/>
+        <v>8.6529123711340201</v>
+      </c>
+      <c r="N12" s="3"/>
+      <c r="O12" s="2">
+        <f t="shared" si="9"/>
+        <v>0.89873331791006006</v>
+      </c>
+      <c r="P12" s="2">
+        <f t="shared" si="10"/>
+        <v>0.88748091986574262</v>
+      </c>
+      <c r="Q12" s="2">
+        <f t="shared" si="11"/>
+        <v>5.3982232177091311E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>252</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="2"/>
+        <v>5.9092000000000002</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="3"/>
+        <v>6.4600000000014689E-3</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="4"/>
+        <v>3.777979999999999</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3">
+        <f t="shared" si="5"/>
+        <v>0.7706400000000011</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" si="6"/>
+        <v>2.2250200000000007</v>
+      </c>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3">
+        <f t="shared" si="7"/>
+        <v>4.5313999999999997</v>
+      </c>
+      <c r="M13" s="3">
+        <f t="shared" si="8"/>
+        <v>10.2225</v>
+      </c>
+      <c r="N13" s="3"/>
+      <c r="O13" s="2">
+        <f t="shared" si="9"/>
+        <v>1.0559262692943967</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="10"/>
+        <v>0.6341359279753237</v>
+      </c>
+      <c r="Q13" s="2">
+        <f t="shared" si="11"/>
+        <v>4.2313508796912072E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>273</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>621.64948453608247</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="2"/>
+        <v>6.7188907216494851</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="3"/>
+        <v>0.7057383505154653</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="4"/>
+        <v>4.6049903092783495</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3">
+        <f t="shared" si="5"/>
+        <v>1.3053822680412381</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="6"/>
+        <v>2.9221334020618563</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3">
+        <f t="shared" si="7"/>
+        <v>5.1332556701030922</v>
+      </c>
+      <c r="M14" s="3">
+        <f t="shared" si="8"/>
+        <v>11.792087628865978</v>
+      </c>
+      <c r="N14" s="3"/>
+      <c r="O14" s="2">
+        <f t="shared" si="9"/>
+        <v>0.82320741591236335</v>
+      </c>
+      <c r="P14" s="2">
+        <f t="shared" si="10"/>
+        <v>0.35420360402147127</v>
+      </c>
+      <c r="Q14" s="2">
+        <f t="shared" si="11"/>
+        <v>2.3088336524122852E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>294</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>643.29896907216494</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="2"/>
+        <v>7.5285814432989691</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="3"/>
+        <v>1.4050167010309291</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="4"/>
+        <v>5.4320006185566996</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3">
+        <f t="shared" si="5"/>
+        <v>1.8401245360824749</v>
+      </c>
+      <c r="J15" s="3">
+        <f t="shared" si="6"/>
+        <v>3.6192468041237116</v>
+      </c>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3">
+        <f t="shared" si="7"/>
+        <v>5.7351113402061848</v>
+      </c>
+      <c r="M15" s="3">
+        <f t="shared" si="8"/>
+        <v>13.361675257731957</v>
+      </c>
+      <c r="N15" s="3"/>
+      <c r="O15" s="2">
+        <f t="shared" si="9"/>
+        <v>0.39354972842347435</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="10"/>
+        <v>0.15144156372921619</v>
+      </c>
+      <c r="Q15" s="2">
+        <f t="shared" si="11"/>
+        <v>8.769839591965497E-8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>315</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>664.94845360824741</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="2"/>
+        <v>8.338272164948453</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="3"/>
+        <v>2.104295051546393</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="4"/>
+        <v>6.2590109278350496</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3">
+        <f t="shared" si="5"/>
+        <v>2.374866804123712</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="6"/>
+        <v>4.3163602061855668</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3">
+        <f t="shared" si="7"/>
+        <v>6.3369670103092774</v>
+      </c>
+      <c r="M16" s="3">
+        <f t="shared" si="8"/>
+        <v>14.931262886597937</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="O16" s="2">
+        <f t="shared" si="9"/>
+        <v>0.11537810797992082</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" si="10"/>
+        <v>4.896241207285517E-2</v>
+      </c>
+      <c r="Q16" s="2">
+        <f t="shared" si="11"/>
+        <v>2.318868163505933E-9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>336</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>686.59793814432987</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="2"/>
+        <v>9.1479628865979379</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="3"/>
+        <v>2.8035734020618568</v>
+      </c>
+      <c r="G17" s="3">
+        <f t="shared" si="4"/>
+        <v>7.0860212371133997</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3">
+        <f t="shared" si="5"/>
+        <v>2.9096090721649488</v>
+      </c>
+      <c r="J17" s="3">
+        <f t="shared" si="6"/>
+        <v>5.0134736082474225</v>
+      </c>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3">
+        <f t="shared" si="7"/>
+        <v>6.93882268041237</v>
+      </c>
+      <c r="M17" s="3">
+        <f t="shared" si="8"/>
+        <v>16.500850515463913</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="O17" s="2">
+        <f t="shared" si="9"/>
+        <v>2.0743471151246917E-2</v>
+      </c>
+      <c r="P17" s="2">
+        <f t="shared" si="10"/>
+        <v>1.1913762710001084E-2</v>
+      </c>
+      <c r="Q17" s="2">
+        <f t="shared" si="11"/>
+        <v>4.2682108802515279E-11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>357</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>708.24742268041246</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="2"/>
+        <v>9.9576536082474263</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" si="3"/>
+        <v>3.5028517525773242</v>
+      </c>
+      <c r="G18" s="3">
+        <f t="shared" si="4"/>
+        <v>7.9130315463917542</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3">
+        <f t="shared" si="5"/>
+        <v>3.4443513402061887</v>
+      </c>
+      <c r="J18" s="3">
+        <f t="shared" si="6"/>
+        <v>5.7105870103092817</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3">
+        <f t="shared" si="7"/>
+        <v>7.5406783505154662</v>
+      </c>
+      <c r="M18" s="3">
+        <f t="shared" si="8"/>
+        <v>18.070438144329902</v>
+      </c>
+      <c r="N18" s="3"/>
+      <c r="O18" s="2">
+        <f t="shared" si="9"/>
+        <v>2.2870396774107324E-3</v>
+      </c>
+      <c r="P18" s="2">
+        <f t="shared" si="10"/>
+        <v>2.1787600197033319E-3</v>
+      </c>
+      <c r="Q18" s="2">
+        <f t="shared" si="11"/>
+        <v>5.4689138398488195E-13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>378</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>729.89690721649481</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="2"/>
+        <v>10.767344329896906</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="3"/>
+        <v>4.2021301030927845</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" si="4"/>
+        <v>8.7400418556700998</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3">
+        <f t="shared" si="5"/>
+        <v>3.9790936082474229</v>
+      </c>
+      <c r="J19" s="3">
+        <f t="shared" si="6"/>
+        <v>6.4077004123711339</v>
+      </c>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3">
+        <f t="shared" si="7"/>
+        <v>8.1425340206185552</v>
+      </c>
+      <c r="M19" s="3">
+        <f t="shared" si="8"/>
+        <v>19.640025773195873</v>
+      </c>
+      <c r="N19" s="3"/>
+      <c r="O19" s="2">
+        <f t="shared" si="9"/>
+        <v>1.5463230015408432E-4</v>
+      </c>
+      <c r="P19" s="2">
+        <f t="shared" si="10"/>
+        <v>2.9937188905645307E-4</v>
+      </c>
+      <c r="Q19" s="2">
+        <f t="shared" si="11"/>
+        <v>4.8779988812652566E-15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>399</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>751.54639175257739</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="2"/>
+        <v>11.577035051546396</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="3"/>
+        <v>4.9014084536082514</v>
+      </c>
+      <c r="G20" s="3">
+        <f t="shared" si="4"/>
+        <v>9.5670521649484552</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3">
+        <f t="shared" si="5"/>
+        <v>4.5138358762886623</v>
+      </c>
+      <c r="J20" s="3">
+        <f t="shared" si="6"/>
+        <v>7.1048138144329922</v>
+      </c>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3">
+        <f t="shared" si="7"/>
+        <v>8.7443896907216505</v>
+      </c>
+      <c r="M20" s="3">
+        <f t="shared" si="8"/>
+        <v>21.209613402061859</v>
+      </c>
+      <c r="N20" s="3"/>
+      <c r="O20" s="2">
+        <f t="shared" si="9"/>
+        <v>6.4115197203944047E-6</v>
+      </c>
+      <c r="P20" s="2">
+        <f t="shared" si="10"/>
+        <v>3.0905103453674714E-5</v>
+      </c>
+      <c r="Q20" s="2">
+        <f t="shared" si="11"/>
+        <v>3.0287798943825876E-17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>420</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>773.19587628865975</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="2"/>
+        <v>12.386725773195876</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="3"/>
+        <v>5.6006868041237121</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" si="4"/>
+        <v>10.394062474226802</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3">
+        <f t="shared" si="5"/>
+        <v>5.0485781443298965</v>
+      </c>
+      <c r="J21" s="3">
+        <f t="shared" si="6"/>
+        <v>7.8019272164948443</v>
+      </c>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3">
+        <f t="shared" si="7"/>
+        <v>9.3462453608247404</v>
+      </c>
+      <c r="M21" s="3">
+        <f t="shared" si="8"/>
+        <v>22.77920103092783</v>
+      </c>
+      <c r="N21" s="3"/>
+      <c r="O21" s="2">
+        <f t="shared" si="9"/>
+        <v>1.6302567166576535E-7</v>
+      </c>
+      <c r="P21" s="2">
+        <f t="shared" si="10"/>
+        <v>2.3969755519380043E-6</v>
+      </c>
+      <c r="Q21" s="2">
+        <f t="shared" si="11"/>
+        <v>1.3091190217792603E-19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>441</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>794.84536082474233</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="2"/>
+        <v>13.196416494845364</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="3"/>
+        <v>6.2999651546391791</v>
+      </c>
+      <c r="G22" s="3">
+        <f t="shared" si="4"/>
+        <v>11.221072783505155</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3">
+        <f t="shared" si="5"/>
+        <v>5.5833204123711369</v>
+      </c>
+      <c r="J22" s="3">
+        <f t="shared" si="6"/>
+        <v>8.4990406185567036</v>
+      </c>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3">
+        <f t="shared" si="7"/>
+        <v>9.9481010309278357</v>
+      </c>
+      <c r="M22" s="3">
+        <f t="shared" si="8"/>
+        <v>24.348788659793819</v>
+      </c>
+      <c r="N22" s="3"/>
+      <c r="O22" s="2">
+        <f t="shared" si="9"/>
+        <v>2.5420568769439531E-9</v>
+      </c>
+      <c r="P22" s="2">
+        <f t="shared" si="10"/>
+        <v>1.3967248013124575E-7</v>
+      </c>
+      <c r="Q22" s="2">
+        <f t="shared" si="11"/>
+        <v>3.938909069675296E-22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>